<commit_message>
debug few mistakes in models
</commit_message>
<xml_diff>
--- a/Final_Results.xlsx
+++ b/Final_Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Academic\Research_Project\ML_models_Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67147AAF-BF5C-4705-9AEB-F263973F6B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9585DB-FA81-44E0-BF97-A612AE261198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="690" yWindow="1005" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,87 +25,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
-  <si>
-    <t>Desease</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
   <si>
     <t>Dataset</t>
   </si>
   <si>
-    <t>Data Type</t>
-  </si>
-  <si>
-    <t>Hypertension</t>
-  </si>
-  <si>
-    <t>Transcriptome</t>
-  </si>
-  <si>
-    <t>Feature Selection</t>
-  </si>
-  <si>
-    <t>Number of Features</t>
-  </si>
-  <si>
     <t>ML Model</t>
   </si>
   <si>
-    <t>Discription About model</t>
-  </si>
-  <si>
-    <t>Accuracy (%)</t>
-  </si>
-  <si>
-    <t>F1 Score (%)</t>
-  </si>
-  <si>
-    <t>Precision (%)</t>
-  </si>
-  <si>
-    <t>Recall (%)</t>
-  </si>
-  <si>
-    <t>Nuber of Miss Labeled Points</t>
-  </si>
-  <si>
     <t>Discription</t>
   </si>
   <si>
-    <t>GSE33463</t>
-  </si>
-  <si>
-    <t>Mutual information</t>
-  </si>
-  <si>
     <t>Random Forest</t>
   </si>
   <si>
-    <t>n = 1000</t>
-  </si>
-  <si>
-    <t>Validation Method</t>
-  </si>
-  <si>
-    <t>test train split 20%</t>
-  </si>
-  <si>
-    <t>instances</t>
-  </si>
-  <si>
-    <t>use instances</t>
-  </si>
-  <si>
-    <t>58/58</t>
-  </si>
-  <si>
-    <t>2_24</t>
-  </si>
-  <si>
-    <t>nave bayes</t>
-  </si>
-  <si>
-    <t>gaussian</t>
+    <t>cv</t>
+  </si>
+  <si>
+    <t>parameters</t>
+  </si>
+  <si>
+    <t>Accurcy</t>
+  </si>
+  <si>
+    <t>STD</t>
+  </si>
+  <si>
+    <t>Hypertension_trans</t>
+  </si>
+  <si>
+    <t>No of features</t>
+  </si>
+  <si>
+    <t>{'max_depth': 90, 'max_features': 3, 'n_estimators': 100}</t>
+  </si>
+  <si>
+    <t>{'max_depth': 80, 'max_features': 2, 'n_estimators': 100}</t>
   </si>
 </sst>
 </file>
@@ -424,168 +379,186 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="5" width="8.85546875" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1"/>
-    <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="9" width="13.7109375" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" customWidth="1"/>
-    <col min="12" max="12" width="11.28515625" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
+    <col min="11" max="11" width="23.42578125" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>87.022000000000006</v>
+      </c>
+      <c r="G2">
+        <v>4.3810000000000002</v>
+      </c>
+      <c r="P2" s="1"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>90.507999999999996</v>
+      </c>
+      <c r="G3">
+        <v>1.2769999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2">
-        <v>140</v>
-      </c>
-      <c r="E2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2">
-        <v>100</v>
-      </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
         <v>20</v>
       </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2">
-        <v>91.667000000000002</v>
-      </c>
-      <c r="L2">
-        <v>90.909000000000006</v>
-      </c>
-      <c r="M2">
-        <v>90.909000000000006</v>
-      </c>
-      <c r="N2">
-        <v>90.909000000000006</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3">
-        <v>140</v>
-      </c>
-      <c r="E3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3">
-        <v>100</v>
-      </c>
-      <c r="H3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3">
-        <v>91.667000000000002</v>
-      </c>
-      <c r="L3">
-        <v>90.909000000000006</v>
-      </c>
-      <c r="M3">
-        <v>84.614999999999995</v>
-      </c>
-      <c r="N3">
-        <v>100</v>
-      </c>
-      <c r="O3" t="s">
-        <v>24</v>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
prepare report for hypertension
</commit_message>
<xml_diff>
--- a/Final_Results.xlsx
+++ b/Final_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Academic\Research_Project\ML_models_Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9585DB-FA81-44E0-BF97-A612AE261198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81985771-DE3B-45B4-9A1D-061B2F9865DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="690" yWindow="1005" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="26">
   <si>
     <t>Dataset</t>
   </si>
@@ -61,6 +61,48 @@
   </si>
   <si>
     <t>{'max_depth': 80, 'max_features': 2, 'n_estimators': 100}</t>
+  </si>
+  <si>
+    <t>{'max_depth': 300, 'max_features': 6, 'n_estimators': 300}</t>
+  </si>
+  <si>
+    <t>{'max_depth': 200, 'max_features': 2, 'n_estimators': 100}</t>
+  </si>
+  <si>
+    <t>{'max_depth': 110, 'max_features': 2, 'n_estimators': 200}</t>
+  </si>
+  <si>
+    <t>{'max_depth': 300, 'max_features': 2, 'n_estimators': 200}</t>
+  </si>
+  <si>
+    <t>{'max_depth': 90, 'max_features': 6, 'n_estimators': 100}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {'max_depth': 80, 'max_features': 2, 'n_estimators': 300}</t>
+  </si>
+  <si>
+    <t>{'max_depth': 150, 'max_features': 4, 'n_estimators': 100}</t>
+  </si>
+  <si>
+    <t>Hypertension_clinical</t>
+  </si>
+  <si>
+    <t>{'max_depth': 200, 'max_features': 2, 'n_estimators': 300}</t>
+  </si>
+  <si>
+    <t>{'max_depth': 150, 'max_features': 2, 'n_estimators': 200}</t>
+  </si>
+  <si>
+    <t>{'max_depth': 110, 'max_features': 4, 'n_estimators': 200}</t>
+  </si>
+  <si>
+    <t>{'max_depth': 100, 'max_features': 3, 'n_estimators': 100}</t>
+  </si>
+  <si>
+    <t>{'max_depth': 200, 'max_features': 2, 'n_estimators': 200}</t>
+  </si>
+  <si>
+    <t>{'max_depth': 90, 'max_features': 2, 'n_estimators': 100}</t>
   </si>
 </sst>
 </file>
@@ -379,19 +421,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" customWidth="1"/>
     <col min="8" max="8" width="19" customWidth="1"/>
     <col min="10" max="10" width="13.7109375" customWidth="1"/>
     <col min="11" max="11" width="23.42578125" customWidth="1"/>
@@ -483,6 +527,18 @@
       <c r="C4" t="s">
         <v>3</v>
       </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>91.379000000000005</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -494,6 +550,18 @@
       <c r="C5" t="s">
         <v>3</v>
       </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>93.102999999999994</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -505,6 +573,18 @@
       <c r="C6" t="s">
         <v>3</v>
       </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>86.206999999999994</v>
+      </c>
+      <c r="G6">
+        <v>3.448</v>
+      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -516,6 +596,18 @@
       <c r="C7" t="s">
         <v>3</v>
       </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>92.24</v>
+      </c>
+      <c r="G7">
+        <v>2.0960000000000001</v>
+      </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -527,16 +619,40 @@
       <c r="C8" t="s">
         <v>3</v>
       </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>93.927000000000007</v>
+      </c>
+      <c r="G8">
+        <v>3.3180000000000001</v>
+      </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>95.69</v>
+      </c>
+      <c r="G9">
+        <v>0.86199999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -544,21 +660,206 @@
         <v>8</v>
       </c>
       <c r="B10">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>95.69</v>
+      </c>
+      <c r="G10">
+        <v>2.5859999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
         <v>20</v>
       </c>
-      <c r="C10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11">
-        <v>50</v>
-      </c>
-      <c r="C11" t="s">
-        <v>3</v>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <v>83.56</v>
+      </c>
+      <c r="G12">
+        <v>6.2480000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <v>82.087000000000003</v>
+      </c>
+      <c r="G13">
+        <v>7.2919999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>83.575999999999993</v>
+      </c>
+      <c r="G14">
+        <v>4.4870000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>83.927000000000007</v>
+      </c>
+      <c r="G15">
+        <v>5.73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16">
+        <v>84.293000000000006</v>
+      </c>
+      <c r="G16">
+        <v>5.2119999999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17">
+        <v>85.578999999999994</v>
+      </c>
+      <c r="G17">
+        <v>5.5369999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18">
+        <v>5</v>
+      </c>
+      <c r="F18">
+        <v>85.051000000000002</v>
+      </c>
+      <c r="G18">
+        <v>5.0339999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>12</v>
+      </c>
+      <c r="C19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <v>84.289000000000001</v>
+      </c>
+      <c r="G19">
+        <v>3.6789999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>